<commit_message>
Big and Small - Races 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/RedMattis/Big and Small - Races - 2894397737/Big and Small - Races - 2894397737.xlsx
+++ b/Data/RedMattis/Big and Small - Races - 2894397737/Big and Small - Races - 2894397737.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\trans\Big and Small - Races - 2894397737\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ACE4A7-8606-4CBB-A1D4-464A8E09C05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4E1FFB-571C-4506-AB71-B13B666736AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="7200" windowWidth="28725" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="2024-04-19_삭제된 노드 목록" sheetId="2" r:id="rId2"/>
+    <sheet name="2024-05-25_삭제된 노드 목록" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1001,12 +1002,51 @@
         </r>
       </text>
     </comment>
+    <comment ref="E84" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004C000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-05-25에 소실되었던 원문이 추가되었습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E85" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-05-25에 소실되었던 원문이 추가되었습니다.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E86" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004E000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-05-25에 소실되었던 원문이 추가되었습니다.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="320">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1035,6 +1075,9 @@
     <t>BS_OgreFaction.label</t>
   </si>
   <si>
+    <t>ogre tribe</t>
+  </si>
+  <si>
     <t>오거 부족</t>
   </si>
   <si>
@@ -1044,924 +1087,970 @@
     <t>BS_OgreFaction.fixedName</t>
   </si>
   <si>
+    <t>Ogre Tribes</t>
+  </si>
+  <si>
+    <t>FactionDef+BS_OgreFaction.leaderTitle</t>
+  </si>
+  <si>
+    <t>BS_OgreFaction.leaderTitle</t>
+  </si>
+  <si>
+    <t>boss</t>
+  </si>
+  <si>
+    <t>보스</t>
+  </si>
+  <si>
+    <t>FactionDef+BS_OgreFaction.description</t>
+  </si>
+  <si>
+    <t>BS_OgreFaction.description</t>
+  </si>
+  <si>
+    <t>These ogres do little more than roam around their settlements in search of fights and food.</t>
+  </si>
+  <si>
+    <t>이 오거는 싸움과 먹이를 찾아 정착지 주변을 배회하는 것 외에는 별다른 활동을 하지 않습니다.</t>
+  </si>
+  <si>
+    <t>FactionDef+BS_LittlePeople.label</t>
+  </si>
+  <si>
+    <t>BS_LittlePeople.label</t>
+  </si>
+  <si>
+    <t>A little people union</t>
+  </si>
+  <si>
+    <t>작은 사람들 연합</t>
+  </si>
+  <si>
+    <t>FactionDef+BS_LittlePeople.description</t>
+  </si>
+  <si>
+    <t>BS_LittlePeople.description</t>
+  </si>
+  <si>
+    <t>A loose union mostly made up of small folk. They are highly distrustful of strangers.</t>
+  </si>
+  <si>
+    <t>대부분 소인들로 구성된 느슨한 연합입니다. 이들은 낯선 사람을 매우 불신합니다.</t>
+  </si>
+  <si>
+    <t>FactionDef+BS_LittlePeople.pawnSingular</t>
+  </si>
+  <si>
+    <t>BS_LittlePeople.pawnSingular</t>
+  </si>
+  <si>
+    <t>smallfolk</t>
+  </si>
+  <si>
+    <t>작은 사람</t>
+  </si>
+  <si>
+    <t>FactionDef+BS_LittlePeople.pawnsPlural</t>
+  </si>
+  <si>
+    <t>BS_LittlePeople.pawnsPlural</t>
+  </si>
+  <si>
+    <t>FactionDef+BS_JotunPlayerColony.label</t>
+  </si>
+  <si>
+    <t>BS_JotunPlayerColony.label</t>
+  </si>
+  <si>
+    <t>Jotun Settlement</t>
+  </si>
+  <si>
+    <t>요툰 정착지</t>
+  </si>
+  <si>
+    <t>FactionDef+BS_JotunPlayerColony.description</t>
+  </si>
+  <si>
+    <t>BS_JotunPlayerColony.description</t>
+  </si>
+  <si>
+    <t>A settlement founded by a jotun exile.</t>
+  </si>
+  <si>
+    <t>요툰 망명자가 세운 정착지입니다.</t>
+  </si>
+  <si>
+    <t>FactionDef+BS_JotunPlayerColony.pawnSingular</t>
+  </si>
+  <si>
+    <t>BS_JotunPlayerColony.pawnSingular</t>
+  </si>
+  <si>
+    <t>settler</t>
+  </si>
+  <si>
+    <t>정착민</t>
+  </si>
+  <si>
+    <t>FactionDef+BS_JotunPlayerColony.pawnsPlural</t>
+  </si>
+  <si>
+    <t>BS_JotunPlayerColony.pawnsPlural</t>
+  </si>
+  <si>
+    <t>settlers</t>
+  </si>
+  <si>
+    <t>정착민들</t>
+  </si>
+  <si>
+    <t>PawnKindDef+BS_Ogre_Chieftain.label</t>
+  </si>
+  <si>
+    <t>PawnKindDef</t>
+  </si>
+  <si>
+    <t>BS_Ogre_Chieftain.label</t>
+  </si>
+  <si>
+    <t>Ogre Tribe Chieftain</t>
+  </si>
+  <si>
+    <t>오거 부족 족장</t>
+  </si>
+  <si>
+    <t>PawnKindDef+BS_DvergrMecha.label</t>
+  </si>
+  <si>
+    <t>BS_DvergrMecha.label</t>
+  </si>
+  <si>
+    <t>Dvergr Mecha</t>
+  </si>
+  <si>
+    <t>드베르그 메카</t>
+  </si>
+  <si>
+    <t>PawnKindDef+BS_NisseMecha.label</t>
+  </si>
+  <si>
+    <t>BS_NisseMecha.label</t>
+  </si>
+  <si>
+    <t>Piloted Mini-Mech</t>
+  </si>
+  <si>
+    <t>조종 미니 기계</t>
+  </si>
+  <si>
+    <t>ScenarioDef+BS_Exiled_Jotun_Adventurer.scenario.name</t>
+  </si>
+  <si>
+    <t>ScenarioDef</t>
+  </si>
+  <si>
+    <t>BS_Exiled_Jotun_Adventurer.scenario.name</t>
+  </si>
+  <si>
+    <t>Exiled Jotun Adventurer</t>
+  </si>
+  <si>
+    <t>추방된 요툰 모험가</t>
+  </si>
+  <si>
+    <t>ScenarioDef+BS_Exiled_Jotun_Adventurer.scenario.description</t>
+  </si>
+  <si>
+    <t>BS_Exiled_Jotun_Adventurer.scenario.description</t>
+  </si>
+  <si>
+    <t>Exiled from your homeland, you must survive in a world that is not your own.</t>
+  </si>
+  <si>
+    <t>고국에서 추방된 당신은 자신의 고향이 아닌 다른 세계에서 살아남아야 합니다.</t>
+  </si>
+  <si>
+    <t>ScenarioDef+BS_Exiled_Jotun_Adventurer.scenario.summary</t>
+  </si>
+  <si>
+    <t>BS_Exiled_Jotun_Adventurer.scenario.summary</t>
+  </si>
+  <si>
+    <t>An exiled jotun adventurer is forced to join forces with some smallfolk</t>
+  </si>
+  <si>
+    <t>추방당한 요툰 모험가가 작은 사람들과 힘을 합치다</t>
+  </si>
+  <si>
+    <t>ScenarioDef+BS_Exiled_Jotun_Adventurer.scenario.parts.2.text</t>
+  </si>
+  <si>
+    <t>BS_Exiled_Jotun_Adventurer.scenario.parts.2.text</t>
+  </si>
+  <si>
+    <t>Exiled from your homeland, you are forced to join forces with some smallfolk to survive</t>
+  </si>
+  <si>
+    <t>고국에서 추방된 당신은 생존을 위해 작은 사람들과 힘을 합쳐야만 합니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+BS_Nisse_Cap.label</t>
+  </si>
+  <si>
+    <t>ThingDef</t>
+  </si>
+  <si>
+    <t>BS_Nisse_Cap.label</t>
+  </si>
+  <si>
+    <t>nisse cap</t>
+  </si>
+  <si>
+    <t>니세 모자</t>
+  </si>
+  <si>
+    <t>ThingDef+BS_Nisse_Cap.description</t>
+  </si>
+  <si>
+    <t>BS_Nisse_Cap.description</t>
+  </si>
+  <si>
+    <t>A cone-shaped hat traditionally worn by Nisse.</t>
+  </si>
+  <si>
+    <t>니세가 전통적으로 착용하는 원뿔 모양의 모자.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Ogre.label</t>
+  </si>
+  <si>
+    <t>XenotypeDef</t>
+  </si>
+  <si>
+    <t>BS_Ogre.label</t>
+  </si>
+  <si>
+    <t>Ogre</t>
+  </si>
+  <si>
+    <t>오거</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Ogre.description</t>
+  </si>
+  <si>
+    <t>BS_Ogre.description</t>
+  </si>
+  <si>
+    <t>The slow lumbering brutes are believed to be a rushed attempt at creating a giant workforce.</t>
+  </si>
+  <si>
+    <t>이 느리게 움직이는 짐승은 거대한 노동력을 급하게 만들려한 시도로 추정됩니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Ogre.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_Ogre.descriptionShort</t>
+  </si>
+  <si>
+    <t>Huge Slow Lumbering brutes.</t>
+  </si>
+  <si>
+    <t>거대하고 느린 육중한 짐승</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_GreatOgre.label</t>
+  </si>
+  <si>
+    <t>BS_GreatOgre.label</t>
+  </si>
+  <si>
+    <t>Great Ogre</t>
+  </si>
+  <si>
+    <t>그레이트 오거</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_GreatOgre.description</t>
+  </si>
+  <si>
+    <t>BS_GreatOgre.description</t>
+  </si>
+  <si>
+    <t>The slow lumbering brutes are believed to either be a failed attempt at creating a giant workforce, or a poor attempt at creating Jotun.</t>
+  </si>
+  <si>
+    <t>이 느리게 움직이는 짐승들은 거대한 노동력을 만들려는 시도가 실패했거나, 요툰을 만들려는 시도가 실패한 것으로 추정됩니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_GreatOgre.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_GreatOgre.descriptionShort</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_FrostJotun.label</t>
+  </si>
+  <si>
+    <t>BS_FrostJotun.label</t>
+  </si>
+  <si>
+    <t>Frost Jotun</t>
+  </si>
+  <si>
+    <t>프로스트 요툰</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_FrostJotun.description</t>
+  </si>
+  <si>
+    <t>BS_FrostJotun.description</t>
+  </si>
+  <si>
+    <t>Towering giants created on a distant world to serve as labourers and soldiers on frozen worlds.</t>
+  </si>
+  <si>
+    <t>얼어붙은 세계에서 노동자와 병사로 일하기 위해 먼 세계에서 만들어진 거인.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_FrostJotun.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_FrostJotun.descriptionShort</t>
+  </si>
+  <si>
+    <t>Towering giants created on a distant world to serve as labourers and soldiers</t>
+  </si>
+  <si>
+    <t>머나먼 세계에서 노동자와 병사로 사용하기 위해 만들어진 거인.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_FireJotun.label</t>
+  </si>
+  <si>
+    <t>BS_FireJotun.label</t>
+  </si>
+  <si>
+    <t>Fire Jotun</t>
+  </si>
+  <si>
+    <t>파이어 요툰</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_FireJotun.description</t>
+  </si>
+  <si>
+    <t>BS_FireJotun.description</t>
+  </si>
+  <si>
+    <t>Towering giants created on a distant world to serve as labourers and soldiers on incredibly hot worlds.</t>
+  </si>
+  <si>
+    <t>엄청나게 뜨거운 세계에서 노동자와 병사로 일하기 위해 먼 세계에서 만들어진 거인.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_FireJotun.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_FireJotun.descriptionShort</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Jotun.label</t>
+  </si>
+  <si>
+    <t>BS_Jotun.label</t>
+  </si>
+  <si>
+    <t>Jotun</t>
+  </si>
+  <si>
+    <t>요툰</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Jotun.description</t>
+  </si>
+  <si>
+    <t>BS_Jotun.description</t>
+  </si>
+  <si>
+    <t>Towering giants created on a distant world to serve as labourers and soldiers.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Jotun.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_Jotun.descriptionShort</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Surtr.label</t>
+  </si>
+  <si>
+    <t>BS_Surtr.label</t>
+  </si>
+  <si>
+    <t>Heir of Surtr</t>
+  </si>
+  <si>
+    <t>수르트의 후계자</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Surtr.description</t>
+  </si>
+  <si>
+    <t>BS_Surtr.description</t>
+  </si>
+  <si>
+    <t>Towering giants created on a distant world to serve as labourers and soldiers on incredibly hot worlds. This one has been enhanced with archites.</t>
+  </si>
+  <si>
+    <t>엄청나게 뜨거운 세계에서 노동자와 병사로 일하기 위해 먼 세계에서 만들어진 거인. 이 거인은 아카이트로 강화되었습니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Surtr.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_Surtr.descriptionShort</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Ymir.label</t>
+  </si>
+  <si>
+    <t>BS_Ymir.label</t>
+  </si>
+  <si>
+    <t>Heir of Aurgelmir</t>
+  </si>
+  <si>
+    <t>아우르겔미르의 후계자</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Ymir.description</t>
+  </si>
+  <si>
+    <t>BS_Ymir.description</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Ymir.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_Ymir.descriptionShort</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_BrokenTitan.label</t>
+  </si>
+  <si>
+    <t>BS_BrokenTitan.label</t>
+  </si>
+  <si>
+    <t>Deteriorating Titan</t>
+  </si>
+  <si>
+    <t>쇠약해진 타이탄</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_BrokenTitan.description</t>
+  </si>
+  <si>
+    <t>BS_BrokenTitan.description</t>
+  </si>
+  <si>
+    <t>This vat-grown titan likely crashed unto the Rim before being properly upgraded. A lack of maintainance has caused its unstable physiology to go berserk on the poor creature.</t>
+  </si>
+  <si>
+    <t>이 배양기에서 자란 타이탄은 제대로 업그레이드되기 전에 변방에 추락한 것으로 보입니다. 관리 부족으로 인해 불안정한 생리가 이 불쌍한 생명체를 광폭하게 만들었습니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_BrokenTitan.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_BrokenTitan.descriptionShort</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Corrupterd_Titan.label</t>
+  </si>
+  <si>
+    <t>BS_Corrupterd_Titan.label</t>
+  </si>
+  <si>
+    <t>corrupted titan</t>
+  </si>
+  <si>
+    <t>타락한 타이탄</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Corrupterd_Titan.description</t>
+  </si>
+  <si>
+    <t>BS_Corrupterd_Titan.description</t>
+  </si>
+  <si>
+    <t>This thing appears to be a titan. The xenogenes and luciferium appears to have gone completely berserk. More a living nanomechanical cancer than a living being at this point. Probably best to put the poor creature out of its missery. Preferably before it tears all of us aparts and consumes us.</t>
+  </si>
+  <si>
+    <t>이건 타이탄처럼 보입니다. 이종유전자와 루시페륨이 완전히 광분한 것 같습니다. 이쯤 되면 생명체라기보다는 살아있는 나노기계 암 덩어리에 가깝습니다. 이 불쌍한 생명체를 없애버리는 게 최선일 것입니다. 가급적이면 우리 모두를 갈기갈기 찢어서 잡아먹기 전에요.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Half_Jotun.label</t>
+  </si>
+  <si>
+    <t>BS_Half_Jotun.label</t>
+  </si>
+  <si>
+    <t>Half Jotun</t>
+  </si>
+  <si>
+    <t>하프 요툰</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Half_Jotun.description</t>
+  </si>
+  <si>
+    <t>BS_Half_Jotun.description</t>
+  </si>
+  <si>
+    <t>Most Half Jotun are believed to be the distant offspring of Jotun.</t>
+  </si>
+  <si>
+    <t>대부분의 하프 요툰은 요툰의 먼 후손으로 추정됩니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Half_Jotun.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_Half_Jotun.descriptionShort</t>
+  </si>
+  <si>
+    <t>Said to be the distant offspring of Jotun.</t>
+  </si>
+  <si>
+    <t>요툰의 먼 후손으로 알려져 있습니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Gnome.label</t>
+  </si>
+  <si>
+    <t>BS_Gnome.label</t>
+  </si>
+  <si>
+    <t>Nisse</t>
+  </si>
+  <si>
+    <t>니세</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Gnome.description</t>
+  </si>
+  <si>
+    <t>BS_Gnome.description</t>
+  </si>
+  <si>
+    <t>Some claim that they were created to do engineering duties on space ships like the Dverger, but their unremarkably affinity for machines indicate otherwise.</t>
+  </si>
+  <si>
+    <t>혹자는 드베르그처럼 우주선에서 엔지니어링 업무를 수행하기 위해 만들어졌다고 주장하지만, 기계에 대한 그들의 유별난 친화력은 그렇지 않다는 것을 보여줍니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Gnome.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_Gnome.descriptionShort</t>
+  </si>
+  <si>
+    <t>They are very short, much like this description.</t>
+  </si>
+  <si>
+    <t>이 설명처럼 매우 짧습니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Dwarf.label</t>
+  </si>
+  <si>
+    <t>BS_Dwarf.label</t>
+  </si>
+  <si>
+    <t>Dvergr</t>
+  </si>
+  <si>
+    <t>드베르그</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Dwarf.description</t>
+  </si>
+  <si>
+    <t>BS_Dwarf.description</t>
+  </si>
+  <si>
+    <t>The popular belief is that they were created to perform engineering duties on space-ships where their small frame would be advantagous. Surprisingly sturdy for their size.</t>
+  </si>
+  <si>
+    <t>작은 체격이 유리한 우주선에서 엔지니어링 임무를 수행하기 위해 만들어졌다는 것이 일반적인 견해입니다. 크기에 비해 놀라울 정도로 튼튼합니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Dwarf.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_Dwarf.descriptionShort</t>
+  </si>
+  <si>
+    <t>Stout and Strong</t>
+  </si>
+  <si>
+    <t>튼튼하고 강인함</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Svartalf.label</t>
+  </si>
+  <si>
+    <t>BS_Svartalf.label</t>
+  </si>
+  <si>
+    <t>Svartalf</t>
+  </si>
+  <si>
+    <t>스바르트알프</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Svartalf.description</t>
+  </si>
+  <si>
+    <t>BS_Svartalf.description</t>
+  </si>
+  <si>
+    <t>Most outlanders that have heard of Svartalfs believe they are some relently malevolent offshot dvergrs. The true nature of Svartalfs is unclear though much due to how rarely they are seen.</t>
+  </si>
+  <si>
+    <t>스바르트알프에 대해 들어본 대부분의 이방인들은 스바르트알프가 악랄한 드워프인 줄로만 알고 있습니다. 스바르트알프의 실체는 워낙 드물게 목격되기 때문에 명확하게 밝혀진 바는 없습니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Svartalf.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_Svartalf.descriptionShort</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Redcap.label</t>
+  </si>
+  <si>
+    <t>BS_Redcap.label</t>
+  </si>
+  <si>
+    <t>Redcap</t>
+  </si>
+  <si>
+    <t>레드캡</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Redcap.description</t>
+  </si>
+  <si>
+    <t>BS_Redcap.description</t>
+  </si>
+  <si>
+    <t>It is hard to say why anyone would engineer something like the Redcaps, but whatever their purpose was they certainly succeeded. Luckily unlike the myth they are based on the Redcaps can in fact be outrun. Usually.\n\nThey are usually seen alone or with their own kind, but sometimes they band together with others when they are desperate for blood.</t>
+  </si>
+  <si>
+    <t>왜 누군가가 레드캡스와 같은 것을 설계했는지 말하기는 어렵지만, 그들의 목적이 무엇이든 간에 그들은 확실히 성공했습니다. 다행히도 신화와는 달리 레드캡스에게서 실제로 도망칠 수 있습니다. 보통은요.\n\n레드캡은 보통 혼자 또는 같은 종족과 함께 나타나지만, 피가 절실할 때는 다른 종족과 함께 뭉치기도 합니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Redcap.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_Redcap.descriptionShort</t>
+  </si>
+  <si>
+    <t>This angry little thing can't possibly be a threat, right?</t>
+  </si>
+  <si>
+    <t>이 화난 꼬마가 위협이 될 수는 없겠죠?</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Hearthguard.label</t>
+  </si>
+  <si>
+    <t>BS_Hearthguard.label</t>
+  </si>
+  <si>
+    <t>Hearthguard</t>
+  </si>
+  <si>
+    <t>허스가드</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Hearthguard.description</t>
+  </si>
+  <si>
+    <t>BS_Hearthguard.description</t>
+  </si>
+  <si>
+    <t>A slow lumbering brutish thing usually created in Dvergr workshops to act as a small warmech. They are usually kept in cryptocaskets to be brought out in case of an attack. They are able to operate on organic food-stuff, and will attempt to process food items to provide for the pilot as well.\n\nMiniature mecha Evangelion?</t>
+  </si>
+  <si>
+    <t>드베르그 작업장에서 작은 워메크 역할을 하는 보통 느리게 움직이는 잔인한 생명체입니다. 이들은 보통 공격이 발생했을 때 꺼내어 사용할 수 있도록 동면관에 보관됩니다. 유기농 식료품을 가공할 수 있으며, 파일럿을 먹여 살리기 위해 식료품 가공도 시도합니다.\n\n미니어처 메카 에반게리온?</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Hearthguard.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_Hearthguard.descriptionShort</t>
+  </si>
+  <si>
+    <t>pilotable semi-organic robot.</t>
+  </si>
+  <si>
+    <t>조종 가능한 반유기체 로봇입니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Hearthdoll.label</t>
+  </si>
+  <si>
+    <t>BS_Hearthdoll.label</t>
+  </si>
+  <si>
+    <t>hearthdoll</t>
+  </si>
+  <si>
+    <t>허스돌</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Hearthdoll.description</t>
+  </si>
+  <si>
+    <t>BS_Hearthdoll.description</t>
+  </si>
+  <si>
+    <t>A slow somewhat clumsy creation usuable made in Dvergr workshops to compensate for the small size of some of their members. They are usually kept in cryptocaskets to be brought out on demand. They are able to operate on organic food-stuff, and will attempt to process food items to provide for the pilot as well.</t>
+  </si>
+  <si>
+    <t>일부 구성원의 작은 크기를 보완하기 위해 드베르그 작업장에서 만든 느리고 다소 어설픈 창조물입니다. 이들은 보통 필요할 때 꺼내어 사용할 수 있도록 동면관에 보관합니다. 이들은 유기농 식료품을 다룰 수 있으며, 파일럿에게 제공할 식료품 가공도 시도할 것입니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Hearthdoll.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_Hearthdoll.descriptionShort</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_PilotableFleshGolem.label</t>
+  </si>
+  <si>
+    <t>BS_PilotableFleshGolem.label</t>
+  </si>
+  <si>
+    <t>flesh golem</t>
+  </si>
+  <si>
+    <t>살점 골렘</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_PilotableFleshGolem.description</t>
+  </si>
+  <si>
+    <t>BS_PilotableFleshGolem.description</t>
+  </si>
+  <si>
+    <t>A partially hollowed-out and somewhat clumsy golem made to impersonate the apperance and abilities human-sized being that is claimed to be created by "magical" means. Only very small xenotypes are able to pilot it.</t>
+  </si>
+  <si>
+    <t>부분적으로 속이 비어 있고 다소 어설픈 골렘으로, 인간 크기의 외모와 능력을 흉내 내기 위해 만들어졌는데, 이 골렘은 "마법적인" 방법으로 만들어졌다고 합니다. 아주 작은 이종족만 조종할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_PilotableFleshGolem.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_PilotableFleshGolem.descriptionShort</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_FleshGolemServant.label</t>
+  </si>
+  <si>
+    <t>BS_FleshGolemServant.label</t>
+  </si>
+  <si>
+    <t>flesh golem servant</t>
+  </si>
+  <si>
+    <t>살점 골렘 서번트</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_FleshGolemServant.description</t>
+  </si>
+  <si>
+    <t>BS_FleshGolemServant.description</t>
+  </si>
+  <si>
+    <t>A flesh golem servant created by unknown means.</t>
+  </si>
+  <si>
+    <t>알 수 없는 방법으로 만들어진 살점 골렘의 하수인입니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_FleshGolemServant.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_FleshGolemServant.descriptionShort</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Troll.label</t>
+  </si>
+  <si>
+    <t>BS_Troll.label</t>
+  </si>
+  <si>
+    <t>Troll</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Troll.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>트롤</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>BS_Troll.description</t>
+  </si>
+  <si>
+    <t>There are stories of old trolls that have grown to the size of mountains. While that is an abusrd claim old trolls are known for being incredibly large. Some say they also grow uglier and uglier with time.</t>
+  </si>
+  <si>
+    <t>산 만하게 자란 늙은 트롤에 대한 이야기가 있습니다. 이는 과장된 주장이지만 오래된 트롤은 엄청나게 큰 것으로 알려져 있습니다. 또한 시간이 지남에 따라 점점 더 추악하게 변한다는 이야기도 있습니다.</t>
+  </si>
+  <si>
+    <t>XenotypeDef+BS_Corrupterd_Titan.descriptionShort</t>
+  </si>
+  <si>
+    <t>BS_Corrupterd_Titan.descriptionShort</t>
+  </si>
+  <si>
+    <t>AHHHHHHHHHHH!</t>
+  </si>
+  <si>
+    <t>BS_NisseGunner.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아아아아아아!</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>mercenary gunner</t>
+  </si>
+  <si>
+    <t>BS_RedcapSlasher.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>용병 사수</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>mercenary slasher</t>
+  </si>
+  <si>
+    <t>BS_LittleBigVillager.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>용병 검사</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>villager</t>
+  </si>
+  <si>
+    <t>FactionDef+BS_JotunPlayerColony.leaderTitle</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>주민</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>BS_JotunPlayerColony.leaderTitle</t>
+  </si>
+  <si>
+    <t>지도자</t>
+  </si>
+  <si>
+    <t>FactionDef+BS_LittlePeople.leaderTitle</t>
+  </si>
+  <si>
+    <t>BS_LittlePeople.leaderTitle</t>
+  </si>
+  <si>
+    <t>고위 의원</t>
+  </si>
+  <si>
+    <t>FactionDef+BS_OgreFaction.pawnsPlural</t>
+  </si>
+  <si>
+    <t>BS_OgreFaction.pawnsPlural</t>
+  </si>
+  <si>
+    <t>부족민</t>
+  </si>
+  <si>
     <t>FactionDef+BS_OgreFaction.pawnSingular</t>
   </si>
   <si>
     <t>BS_OgreFaction.pawnSingular</t>
   </si>
   <si>
-    <t>부족민</t>
-  </si>
-  <si>
-    <t>FactionDef+BS_OgreFaction.pawnsPlural</t>
-  </si>
-  <si>
-    <t>BS_OgreFaction.pawnsPlural</t>
-  </si>
-  <si>
-    <t>FactionDef+BS_OgreFaction.leaderTitle</t>
-  </si>
-  <si>
-    <t>BS_OgreFaction.leaderTitle</t>
-  </si>
-  <si>
-    <t>보스</t>
-  </si>
-  <si>
-    <t>FactionDef+BS_OgreFaction.description</t>
-  </si>
-  <si>
-    <t>BS_OgreFaction.description</t>
-  </si>
-  <si>
-    <t>이 오거는 싸움과 먹이를 찾아 정착지 주변을 배회하는 것 외에는 별다른 활동을 하지 않습니다.</t>
-  </si>
-  <si>
-    <t>FactionDef+BS_LittlePeople.label</t>
-  </si>
-  <si>
-    <t>BS_LittlePeople.label</t>
-  </si>
-  <si>
-    <t>작은 사람들 연합</t>
-  </si>
-  <si>
-    <t>FactionDef+BS_LittlePeople.description</t>
-  </si>
-  <si>
-    <t>BS_LittlePeople.description</t>
-  </si>
-  <si>
-    <t>대부분 소인들로 구성된 느슨한 연합입니다. 이들은 낯선 사람을 매우 불신합니다.</t>
-  </si>
-  <si>
-    <t>FactionDef+BS_LittlePeople.pawnSingular</t>
-  </si>
-  <si>
-    <t>BS_LittlePeople.pawnSingular</t>
-  </si>
-  <si>
-    <t>작은 사람</t>
-  </si>
-  <si>
-    <t>FactionDef+BS_LittlePeople.pawnsPlural</t>
-  </si>
-  <si>
-    <t>BS_LittlePeople.pawnsPlural</t>
-  </si>
-  <si>
-    <t>FactionDef+BS_LittlePeople.leaderTitle</t>
-  </si>
-  <si>
-    <t>BS_LittlePeople.leaderTitle</t>
-  </si>
-  <si>
-    <t>고위 의원</t>
-  </si>
-  <si>
-    <t>FactionDef+BS_JotunPlayerColony.label</t>
-  </si>
-  <si>
-    <t>BS_JotunPlayerColony.label</t>
-  </si>
-  <si>
-    <t>요툰 정착지</t>
-  </si>
-  <si>
-    <t>FactionDef+BS_JotunPlayerColony.description</t>
-  </si>
-  <si>
-    <t>BS_JotunPlayerColony.description</t>
-  </si>
-  <si>
-    <t>요툰 망명자가 세운 정착지입니다.</t>
-  </si>
-  <si>
-    <t>FactionDef+BS_JotunPlayerColony.pawnSingular</t>
-  </si>
-  <si>
-    <t>BS_JotunPlayerColony.pawnSingular</t>
-  </si>
-  <si>
-    <t>정착민</t>
-  </si>
-  <si>
-    <t>FactionDef+BS_JotunPlayerColony.pawnsPlural</t>
-  </si>
-  <si>
-    <t>BS_JotunPlayerColony.pawnsPlural</t>
-  </si>
-  <si>
-    <t>정착민들</t>
-  </si>
-  <si>
-    <t>FactionDef+BS_JotunPlayerColony.leaderTitle</t>
-  </si>
-  <si>
-    <t>BS_JotunPlayerColony.leaderTitle</t>
-  </si>
-  <si>
-    <t>지도자</t>
-  </si>
-  <si>
-    <t>PawnKindDef+BS_Ogre_Chieftain.label</t>
-  </si>
-  <si>
-    <t>PawnKindDef</t>
-  </si>
-  <si>
-    <t>BS_Ogre_Chieftain.label</t>
-  </si>
-  <si>
-    <t>오거 부족 족장</t>
-  </si>
-  <si>
-    <t>PawnKindDef+BS_DvergrMecha.label</t>
-  </si>
-  <si>
-    <t>BS_DvergrMecha.label</t>
-  </si>
-  <si>
-    <t>드베르그 메카</t>
-  </si>
-  <si>
-    <t>PawnKindDef+BS_NisseMecha.label</t>
-  </si>
-  <si>
-    <t>BS_NisseMecha.label</t>
-  </si>
-  <si>
-    <t>조종 미니 기계</t>
+    <t>ScenarioDef+BS_Exiled_Jotun_Adventurer.description</t>
+  </si>
+  <si>
+    <t>BS_Exiled_Jotun_Adventurer.description</t>
   </si>
   <si>
     <t>ScenarioDef+BS_Exiled_Jotun_Adventurer.label</t>
   </si>
   <si>
-    <t>ScenarioDef</t>
-  </si>
-  <si>
     <t>BS_Exiled_Jotun_Adventurer.label</t>
   </si>
   <si>
-    <t>추방된 요툰 모험가</t>
-  </si>
-  <si>
-    <t>ScenarioDef+BS_Exiled_Jotun_Adventurer.description</t>
-  </si>
-  <si>
-    <t>BS_Exiled_Jotun_Adventurer.description</t>
-  </si>
-  <si>
-    <t>고국에서 추방된 당신은 자신의 고향이 아닌 다른 세계에서 살아남아야 합니다.</t>
-  </si>
-  <si>
-    <t>ScenarioDef+BS_Exiled_Jotun_Adventurer.scenario.name</t>
-  </si>
-  <si>
-    <t>BS_Exiled_Jotun_Adventurer.scenario.name</t>
-  </si>
-  <si>
-    <t>ScenarioDef+BS_Exiled_Jotun_Adventurer.scenario.description</t>
-  </si>
-  <si>
-    <t>BS_Exiled_Jotun_Adventurer.scenario.description</t>
-  </si>
-  <si>
-    <t>ScenarioDef+BS_Exiled_Jotun_Adventurer.scenario.summary</t>
-  </si>
-  <si>
-    <t>BS_Exiled_Jotun_Adventurer.scenario.summary</t>
-  </si>
-  <si>
-    <t>추방당한 요툰 모험가가 작은 사람들과 힘을 합치다</t>
-  </si>
-  <si>
-    <t>ScenarioDef+BS_Exiled_Jotun_Adventurer.scenario.parts.2.text</t>
-  </si>
-  <si>
-    <t>BS_Exiled_Jotun_Adventurer.scenario.parts.2.text</t>
-  </si>
-  <si>
-    <t>고국에서 추방된 당신은 생존을 위해 작은 사람들과 힘을 합쳐야만 합니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+BS_Nisse_Cap.label</t>
-  </si>
-  <si>
-    <t>ThingDef</t>
-  </si>
-  <si>
-    <t>BS_Nisse_Cap.label</t>
-  </si>
-  <si>
-    <t>니세 모자</t>
-  </si>
-  <si>
-    <t>ThingDef+BS_Nisse_Cap.description</t>
-  </si>
-  <si>
-    <t>BS_Nisse_Cap.description</t>
-  </si>
-  <si>
-    <t>니세가 전통적으로 착용하는 원뿔 모양의 모자.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Ogre.label</t>
-  </si>
-  <si>
-    <t>XenotypeDef</t>
-  </si>
-  <si>
-    <t>BS_Ogre.label</t>
-  </si>
-  <si>
-    <t>오거</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Ogre.description</t>
-  </si>
-  <si>
-    <t>BS_Ogre.description</t>
-  </si>
-  <si>
-    <t>이 느리게 움직이는 짐승은 거대한 노동력을 급하게 만들려한 시도로 추정됩니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Ogre.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_Ogre.descriptionShort</t>
-  </si>
-  <si>
-    <t>거대하고 느린 육중한 짐승</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_GreatOgre.label</t>
-  </si>
-  <si>
-    <t>BS_GreatOgre.label</t>
-  </si>
-  <si>
-    <t>그레이트 오거</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_GreatOgre.description</t>
-  </si>
-  <si>
-    <t>BS_GreatOgre.description</t>
-  </si>
-  <si>
-    <t>이 느리게 움직이는 짐승들은 거대한 노동력을 만들려는 시도가 실패했거나, 요툰을 만들려는 시도가 실패한 것으로 추정됩니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_GreatOgre.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_GreatOgre.descriptionShort</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_FrostJotun.label</t>
-  </si>
-  <si>
-    <t>BS_FrostJotun.label</t>
-  </si>
-  <si>
-    <t>프로스트 요툰</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_FrostJotun.description</t>
-  </si>
-  <si>
-    <t>BS_FrostJotun.description</t>
-  </si>
-  <si>
-    <t>얼어붙은 세계에서 노동자와 병사로 일하기 위해 먼 세계에서 만들어진 거인.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_FrostJotun.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_FrostJotun.descriptionShort</t>
-  </si>
-  <si>
-    <t>머나먼 세계에서 노동자와 병사로 사용하기 위해 만들어진 거인.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_FireJotun.label</t>
-  </si>
-  <si>
-    <t>BS_FireJotun.label</t>
-  </si>
-  <si>
-    <t>파이어 요툰</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_FireJotun.description</t>
-  </si>
-  <si>
-    <t>BS_FireJotun.description</t>
-  </si>
-  <si>
-    <t>엄청나게 뜨거운 세계에서 노동자와 병사로 일하기 위해 먼 세계에서 만들어진 거인.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_FireJotun.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_FireJotun.descriptionShort</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Jotun.label</t>
-  </si>
-  <si>
-    <t>BS_Jotun.label</t>
-  </si>
-  <si>
-    <t>요툰</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Jotun.description</t>
-  </si>
-  <si>
-    <t>BS_Jotun.description</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Jotun.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_Jotun.descriptionShort</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Surtr.label</t>
-  </si>
-  <si>
-    <t>BS_Surtr.label</t>
-  </si>
-  <si>
-    <t>수르트의 후계자</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Surtr.description</t>
-  </si>
-  <si>
-    <t>BS_Surtr.description</t>
-  </si>
-  <si>
-    <t>엄청나게 뜨거운 세계에서 노동자와 병사로 일하기 위해 먼 세계에서 만들어진 거인. 이 거인은 아카이트로 강화되었습니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Surtr.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_Surtr.descriptionShort</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Ymir.label</t>
-  </si>
-  <si>
-    <t>BS_Ymir.label</t>
-  </si>
-  <si>
-    <t>아우르겔미르의 후계자</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Ymir.description</t>
-  </si>
-  <si>
-    <t>BS_Ymir.description</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Ymir.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_Ymir.descriptionShort</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_BrokenTitan.label</t>
-  </si>
-  <si>
-    <t>BS_BrokenTitan.label</t>
-  </si>
-  <si>
-    <t>쇠약해진 타이탄</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_BrokenTitan.description</t>
-  </si>
-  <si>
-    <t>BS_BrokenTitan.description</t>
-  </si>
-  <si>
-    <t>이 배양기에서 자란 타이탄은 제대로 업그레이드되기 전에 변방에 추락한 것으로 보입니다. 관리 부족으로 인해 불안정한 생리가 이 불쌍한 생명체를 광폭하게 만들었습니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_BrokenTitan.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_BrokenTitan.descriptionShort</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Corrupterd_Titan.label</t>
-  </si>
-  <si>
-    <t>BS_Corrupterd_Titan.label</t>
-  </si>
-  <si>
-    <t>타락한 타이탄</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Corrupterd_Titan.description</t>
-  </si>
-  <si>
-    <t>BS_Corrupterd_Titan.description</t>
-  </si>
-  <si>
-    <t>이건 타이탄처럼 보입니다. 이종유전자와 루시페륨이 완전히 광분한 것 같습니다. 이쯤 되면 생명체라기보다는 살아있는 나노기계 암 덩어리에 가깝습니다. 이 불쌍한 생명체를 없애버리는 게 최선일 것입니다. 가급적이면 우리 모두를 갈기갈기 찢어서 잡아먹기 전에요.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Half_Jotun.label</t>
-  </si>
-  <si>
-    <t>BS_Half_Jotun.label</t>
-  </si>
-  <si>
-    <t>하프 요툰</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Half_Jotun.description</t>
-  </si>
-  <si>
-    <t>BS_Half_Jotun.description</t>
-  </si>
-  <si>
-    <t>대부분의 하프 요툰은 요툰의 먼 후손으로 추정됩니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Half_Jotun.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_Half_Jotun.descriptionShort</t>
-  </si>
-  <si>
-    <t>요툰의 먼 후손으로 알려져 있습니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Gnome.label</t>
-  </si>
-  <si>
-    <t>BS_Gnome.label</t>
-  </si>
-  <si>
-    <t>니세</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Gnome.description</t>
-  </si>
-  <si>
-    <t>BS_Gnome.description</t>
-  </si>
-  <si>
-    <t>혹자는 드베르그처럼 우주선에서 엔지니어링 업무를 수행하기 위해 만들어졌다고 주장하지만, 기계에 대한 그들의 유별난 친화력은 그렇지 않다는 것을 보여줍니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Gnome.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_Gnome.descriptionShort</t>
-  </si>
-  <si>
-    <t>이 설명처럼 매우 짧습니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Dwarf.label</t>
-  </si>
-  <si>
-    <t>BS_Dwarf.label</t>
-  </si>
-  <si>
-    <t>드베르그</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Dwarf.description</t>
-  </si>
-  <si>
-    <t>BS_Dwarf.description</t>
-  </si>
-  <si>
-    <t>작은 체격이 유리한 우주선에서 엔지니어링 임무를 수행하기 위해 만들어졌다는 것이 일반적인 견해입니다. 크기에 비해 놀라울 정도로 튼튼합니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Dwarf.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_Dwarf.descriptionShort</t>
-  </si>
-  <si>
-    <t>튼튼하고 강인함</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Svartalf.label</t>
-  </si>
-  <si>
-    <t>BS_Svartalf.label</t>
-  </si>
-  <si>
-    <t>스바르트알프</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Svartalf.description</t>
-  </si>
-  <si>
-    <t>BS_Svartalf.description</t>
-  </si>
-  <si>
-    <t>스바르트알프에 대해 들어본 대부분의 이방인들은 스바르트알프가 악랄한 드워프인 줄로만 알고 있습니다. 스바르트알프의 실체는 워낙 드물게 목격되기 때문에 명확하게 밝혀진 바는 없습니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Svartalf.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_Svartalf.descriptionShort</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Redcap.label</t>
-  </si>
-  <si>
-    <t>BS_Redcap.label</t>
-  </si>
-  <si>
-    <t>레드캡</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Redcap.description</t>
-  </si>
-  <si>
-    <t>BS_Redcap.description</t>
-  </si>
-  <si>
-    <t>왜 누군가가 레드캡스와 같은 것을 설계했는지 말하기는 어렵지만, 그들의 목적이 무엇이든 간에 그들은 확실히 성공했습니다. 다행히도 신화와는 달리 레드캡스에게서 실제로 도망칠 수 있습니다. 보통은요.\n\n레드캡은 보통 혼자 또는 같은 종족과 함께 나타나지만, 피가 절실할 때는 다른 종족과 함께 뭉치기도 합니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Redcap.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_Redcap.descriptionShort</t>
-  </si>
-  <si>
-    <t>이 화난 꼬마가 위협이 될 수는 없겠죠?</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Hearthguard.label</t>
-  </si>
-  <si>
-    <t>BS_Hearthguard.label</t>
-  </si>
-  <si>
-    <t>허스가드</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Hearthguard.description</t>
-  </si>
-  <si>
-    <t>BS_Hearthguard.description</t>
-  </si>
-  <si>
-    <t>드베르그 작업장에서 작은 워메크 역할을 하는 보통 느리게 움직이는 잔인한 생명체입니다. 이들은 보통 공격이 발생했을 때 꺼내어 사용할 수 있도록 동면관에 보관됩니다. 유기농 식료품을 가공할 수 있으며, 파일럿을 먹여 살리기 위해 식료품 가공도 시도합니다.\n\n미니어처 메카 에반게리온?</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Hearthguard.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_Hearthguard.descriptionShort</t>
-  </si>
-  <si>
-    <t>조종 가능한 반유기체 로봇입니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Hearthdoll.label</t>
-  </si>
-  <si>
-    <t>BS_Hearthdoll.label</t>
-  </si>
-  <si>
-    <t>허스돌</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Hearthdoll.description</t>
-  </si>
-  <si>
-    <t>BS_Hearthdoll.description</t>
-  </si>
-  <si>
-    <t>일부 구성원의 작은 크기를 보완하기 위해 드베르그 작업장에서 만든 느리고 다소 어설픈 창조물입니다. 이들은 보통 필요할 때 꺼내어 사용할 수 있도록 동면관에 보관합니다. 이들은 유기농 식료품을 다룰 수 있으며, 파일럿에게 제공할 식료품 가공도 시도할 것입니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Hearthdoll.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_Hearthdoll.descriptionShort</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_PilotableFleshGolem.label</t>
-  </si>
-  <si>
-    <t>BS_PilotableFleshGolem.label</t>
-  </si>
-  <si>
-    <t>살점 골렘</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_PilotableFleshGolem.description</t>
-  </si>
-  <si>
-    <t>BS_PilotableFleshGolem.description</t>
-  </si>
-  <si>
-    <t>부분적으로 속이 비어 있고 다소 어설픈 골렘으로, 인간 크기의 외모와 능력을 흉내 내기 위해 만들어졌는데, 이 골렘은 "마법적인" 방법으로 만들어졌다고 합니다. 아주 작은 이종족만 조종할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_PilotableFleshGolem.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_PilotableFleshGolem.descriptionShort</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_FleshGolemServant.label</t>
-  </si>
-  <si>
-    <t>BS_FleshGolemServant.label</t>
-  </si>
-  <si>
-    <t>살점 골렘 서번트</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_FleshGolemServant.description</t>
-  </si>
-  <si>
-    <t>BS_FleshGolemServant.description</t>
-  </si>
-  <si>
-    <t>알 수 없는 방법으로 만들어진 살점 골렘의 하수인입니다.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_FleshGolemServant.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_FleshGolemServant.descriptionShort</t>
-  </si>
-  <si>
-    <t>ogre tribe</t>
-  </si>
-  <si>
-    <t>Ogre Tribes</t>
-  </si>
-  <si>
-    <t>boss</t>
-  </si>
-  <si>
-    <t>These ogres do little more than roam around their settlements in search of fights and food.</t>
-  </si>
-  <si>
-    <t>A little people union</t>
-  </si>
-  <si>
-    <t>A loose union mostly made up of small folk. They are highly distrustful of strangers.</t>
-  </si>
-  <si>
-    <t>smallfolk</t>
-  </si>
-  <si>
-    <t>Jotun Settlement</t>
-  </si>
-  <si>
-    <t>A settlement founded by a jotun exile.</t>
-  </si>
-  <si>
-    <t>settler</t>
-  </si>
-  <si>
-    <t>settlers</t>
-  </si>
-  <si>
-    <t>Ogre Tribe Chieftain</t>
-  </si>
-  <si>
-    <t>Dvergr Mecha</t>
-  </si>
-  <si>
-    <t>Piloted Mini-Mech</t>
-  </si>
-  <si>
-    <t>Exiled Jotun Adventurer</t>
-  </si>
-  <si>
-    <t>Exiled from your homeland, you must survive in a world that is not your own.</t>
-  </si>
-  <si>
-    <t>An exiled jotun adventurer is forced to join forces with some smallfolk</t>
-  </si>
-  <si>
-    <t>Exiled from your homeland, you are forced to join forces with some smallfolk to survive</t>
-  </si>
-  <si>
-    <t>nisse cap</t>
-  </si>
-  <si>
-    <t>A cone-shaped hat traditionally worn by Nisse.</t>
-  </si>
-  <si>
-    <t>Ogre</t>
-  </si>
-  <si>
-    <t>The slow lumbering brutes are believed to be a rushed attempt at creating a giant workforce.</t>
-  </si>
-  <si>
-    <t>Huge Slow Lumbering brutes.</t>
-  </si>
-  <si>
-    <t>Great Ogre</t>
-  </si>
-  <si>
-    <t>The slow lumbering brutes are believed to either be a failed attempt at creating a giant workforce, or a poor attempt at creating Jotun.</t>
-  </si>
-  <si>
-    <t>Frost Jotun</t>
-  </si>
-  <si>
-    <t>Towering giants created on a distant world to serve as labourers and soldiers on frozen worlds.</t>
-  </si>
-  <si>
-    <t>Towering giants created on a distant world to serve as labourers and soldiers</t>
-  </si>
-  <si>
-    <t>Fire Jotun</t>
-  </si>
-  <si>
-    <t>Towering giants created on a distant world to serve as labourers and soldiers on incredibly hot worlds.</t>
-  </si>
-  <si>
-    <t>Jotun</t>
-  </si>
-  <si>
-    <t>Towering giants created on a distant world to serve as labourers and soldiers.</t>
-  </si>
-  <si>
-    <t>Heir of Surtr</t>
-  </si>
-  <si>
-    <t>Towering giants created on a distant world to serve as labourers and soldiers on incredibly hot worlds. This one has been enhanced with archites.</t>
-  </si>
-  <si>
-    <t>Heir of Aurgelmir</t>
-  </si>
-  <si>
-    <t>Deteriorating Titan</t>
-  </si>
-  <si>
-    <t>This vat-grown titan likely crashed unto the Rim before being properly upgraded. A lack of maintainance has caused its unstable physiology to go berserk on the poor creature.</t>
-  </si>
-  <si>
-    <t>corrupted titan</t>
-  </si>
-  <si>
-    <t>This thing appears to be a titan. The xenogenes and luciferium appears to have gone completely berserk. More a living nanomechanical cancer than a living being at this point. Probably best to put the poor creature out of its missery. Preferably before it tears all of us aparts and consumes us.</t>
-  </si>
-  <si>
-    <t>Half Jotun</t>
-  </si>
-  <si>
-    <t>Most Half Jotun are believed to be the distant offspring of Jotun.</t>
-  </si>
-  <si>
-    <t>Said to be the distant offspring of Jotun.</t>
-  </si>
-  <si>
-    <t>Nisse</t>
-  </si>
-  <si>
-    <t>Some claim that they were created to do engineering duties on space ships like the Dverger, but their unremarkably affinity for machines indicate otherwise.</t>
-  </si>
-  <si>
-    <t>They are very short, much like this description.</t>
-  </si>
-  <si>
-    <t>Dvergr</t>
-  </si>
-  <si>
-    <t>The popular belief is that they were created to perform engineering duties on space-ships where their small frame would be advantagous. Surprisingly sturdy for their size.</t>
-  </si>
-  <si>
-    <t>Stout and Strong</t>
-  </si>
-  <si>
-    <t>Svartalf</t>
-  </si>
-  <si>
-    <t>Most outlanders that have heard of Svartalfs believe they are some relently malevolent offshot dvergrs. The true nature of Svartalfs is unclear though much due to how rarely they are seen.</t>
-  </si>
-  <si>
-    <t>Redcap</t>
-  </si>
-  <si>
-    <t>It is hard to say why anyone would engineer something like the Redcaps, but whatever their purpose was they certainly succeeded. Luckily unlike the myth they are based on the Redcaps can in fact be outrun. Usually.\n\nThey are usually seen alone or with their own kind, but sometimes they band together with others when they are desperate for blood.</t>
-  </si>
-  <si>
-    <t>This angry little thing can't possibly be a threat, right?</t>
-  </si>
-  <si>
-    <t>Hearthguard</t>
-  </si>
-  <si>
-    <t>A slow lumbering brutish thing usually created in Dvergr workshops to act as a small warmech. They are usually kept in cryptocaskets to be brought out in case of an attack. They are able to operate on organic food-stuff, and will attempt to process food items to provide for the pilot as well.\n\nMiniature mecha Evangelion?</t>
-  </si>
-  <si>
-    <t>pilotable semi-organic robot.</t>
-  </si>
-  <si>
-    <t>hearthdoll</t>
-  </si>
-  <si>
-    <t>A slow somewhat clumsy creation usuable made in Dvergr workshops to compensate for the small size of some of their members. They are usually kept in cryptocaskets to be brought out on demand. They are able to operate on organic food-stuff, and will attempt to process food items to provide for the pilot as well.</t>
-  </si>
-  <si>
-    <t>flesh golem</t>
-  </si>
-  <si>
-    <t>A partially hollowed-out and somewhat clumsy golem made to impersonate the apperance and abilities human-sized being that is claimed to be created by "magical" means. Only very small xenotypes are able to pilot it.</t>
-  </si>
-  <si>
-    <t>flesh golem servant</t>
-  </si>
-  <si>
-    <t>A flesh golem servant created by unknown means.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Troll.label</t>
-  </si>
-  <si>
-    <t>BS_Troll.label</t>
-  </si>
-  <si>
-    <t>Troll</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Troll.description</t>
-  </si>
-  <si>
-    <t>BS_Troll.description</t>
-  </si>
-  <si>
-    <t>There are stories of old trolls that have grown to the size of mountains. While that is an abusrd claim old trolls are known for being incredibly large. Some say they also grow uglier and uglier with time.</t>
-  </si>
-  <si>
-    <t>XenotypeDef+BS_Corrupterd_Titan.descriptionShort</t>
-  </si>
-  <si>
-    <t>BS_Corrupterd_Titan.descriptionShort</t>
-  </si>
-  <si>
-    <t>AHHHHHHHHHHH!</t>
-  </si>
-  <si>
-    <t>트롤</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>산 만하게 자란 늙은 트롤에 대한 이야기가 있습니다. 이는 과장된 주장이지만 오래된 트롤은 엄청나게 큰 것으로 알려져 있습니다. 또한 시간이 지남에 따라 점점 더 추악하게 변한다는 이야기도 있습니다.</t>
-  </si>
-  <si>
-    <t>아아아아아아!</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BS_NisseGunner.label</t>
-  </si>
-  <si>
-    <t>BS_RedcapSlasher.label</t>
-  </si>
-  <si>
-    <t>BS_LittleBigVillager.label</t>
-  </si>
-  <si>
-    <t>mercenary gunner</t>
-  </si>
-  <si>
-    <t>mercenary slasher</t>
-  </si>
-  <si>
-    <t>villager</t>
-  </si>
-  <si>
-    <t>용병 사수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>용병 검사</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>주민</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>prime councilor</t>
+  </si>
+  <si>
+    <t>tribespeople</t>
+  </si>
+  <si>
+    <t>tribesman</t>
   </si>
 </sst>
 </file>
@@ -2331,10 +2420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86 C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2378,75 +2467,75 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>234</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>235</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>236</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>25</v>
@@ -2463,58 +2552,58 @@
         <v>27</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>239</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>240</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>241</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>39</v>
@@ -2531,44 +2620,44 @@
         <v>41</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>242</v>
+        <v>42</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>243</v>
+        <v>46</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>244</v>
+        <v>50</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2582,1098 +2671,1098 @@
         <v>54</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>245</v>
+        <v>55</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>246</v>
+        <v>59</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>247</v>
+        <v>63</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>250</v>
+        <v>76</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>251</v>
+        <v>80</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>252</v>
+        <v>85</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>253</v>
+        <v>89</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>254</v>
+        <v>94</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>255</v>
+        <v>98</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>256</v>
+        <v>102</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>257</v>
+        <v>106</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>258</v>
+        <v>110</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>259</v>
+        <v>116</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>260</v>
+        <v>120</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>261</v>
+        <v>124</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>262</v>
+        <v>128</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>263</v>
+        <v>132</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>261</v>
+        <v>124</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>264</v>
+        <v>138</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>261</v>
+        <v>124</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>266</v>
+        <v>147</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>267</v>
+        <v>151</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>261</v>
+        <v>124</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>268</v>
+        <v>157</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>267</v>
+        <v>151</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>261</v>
+        <v>124</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>269</v>
+        <v>165</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>270</v>
+        <v>169</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>261</v>
+        <v>124</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>271</v>
+        <v>175</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>272</v>
+        <v>179</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>273</v>
+        <v>183</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>274</v>
+        <v>187</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>162</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>275</v>
+        <v>191</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>276</v>
+        <v>195</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>277</v>
+        <v>199</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>278</v>
+        <v>203</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>174</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>279</v>
+        <v>207</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>179</v>
+        <v>210</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>280</v>
+        <v>211</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>180</v>
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>182</v>
+        <v>214</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>281</v>
+        <v>215</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>183</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>184</v>
+        <v>217</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>185</v>
+        <v>218</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>187</v>
+        <v>221</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>188</v>
+        <v>222</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>283</v>
+        <v>223</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>189</v>
+        <v>224</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>190</v>
+        <v>225</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>191</v>
+        <v>226</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>281</v>
+        <v>215</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>183</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>192</v>
+        <v>227</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>193</v>
+        <v>228</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>284</v>
+        <v>229</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>194</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>285</v>
+        <v>233</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>197</v>
+        <v>234</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>198</v>
+        <v>235</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>199</v>
+        <v>236</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>286</v>
+        <v>237</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>200</v>
+        <v>238</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>201</v>
+        <v>239</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>202</v>
+        <v>240</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>287</v>
+        <v>241</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>203</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>204</v>
+        <v>243</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>288</v>
+        <v>245</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>206</v>
+        <v>246</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>207</v>
+        <v>247</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>208</v>
+        <v>248</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>289</v>
+        <v>249</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>210</v>
+        <v>251</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>211</v>
+        <v>252</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>212</v>
+        <v>254</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>213</v>
+        <v>255</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>214</v>
+        <v>256</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>215</v>
+        <v>258</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>216</v>
+        <v>259</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>217</v>
+        <v>260</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>289</v>
+        <v>249</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>218</v>
+        <v>261</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>219</v>
+        <v>262</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>292</v>
+        <v>263</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>220</v>
+        <v>264</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>221</v>
+        <v>265</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>222</v>
+        <v>266</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>293</v>
+        <v>267</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>223</v>
+        <v>268</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>224</v>
+        <v>269</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>289</v>
+        <v>249</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>226</v>
+        <v>271</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>227</v>
+        <v>272</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>294</v>
+        <v>273</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>228</v>
+        <v>274</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>229</v>
+        <v>275</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>230</v>
+        <v>276</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>231</v>
+        <v>278</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>232</v>
+        <v>279</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>233</v>
+        <v>280</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>289</v>
+        <v>249</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -3681,13 +3770,13 @@
         <v>53</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -3695,13 +3784,13 @@
         <v>53</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -3709,69 +3798,64 @@
         <v>53</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>49</v>
+        <v>305</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>50</v>
+        <v>306</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>51</v>
+        <v>307</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>34</v>
+        <v>308</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>35</v>
+        <v>309</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>36</v>
+        <v>310</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>15</v>
+        <v>311</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>16</v>
+        <v>312</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>14</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -3786,11 +3870,12 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F7"/>
+      <selection activeCell="A4" sqref="A4 A4:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3814,107 +3899,158 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
+        <v>314</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>315</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>64</v>
+        <v>316</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>301</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>303</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>51</v>
+        <v>304</v>
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>305</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>306</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>307</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>308</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>309</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>310</v>
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>311</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>312</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>310</v>
       </c>
       <c r="G7" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G2" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>